<commit_message>
feat: Update COVAX_AGG package for DHIS2 v2.30 & 2.33
</commit_message>
<xml_diff>
--- a/metadata/COVAX_AGG/COVAX_AGG_COMPLETE_V1_DHIS2.30/reference.xlsx
+++ b/metadata/COVAX_AGG/COVAX_AGG_COMPLETE_V1_DHIS2.30/reference.xlsx
@@ -503,7 +503,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAX_AGG_COMPLETE_V1.0_DHIS2.30_2021-01-28T18:52</v>
+        <v>COVAX_AGG_COMPLETE_V1.0_DHIS2.30_2021-01-29T11:09</v>
       </c>
     </row>
   </sheetData>
@@ -2786,7 +2786,7 @@
         <v>CVX_OPENING_BALANCE_SYRINGES_WITH_ NEEDLE_1ML</v>
       </c>
       <c r="E2" s="4" t="str">
-        <v>Opening balance equals the physical 'stock on hand count' of the previous period</v>
+        <v>Opening balance equals the physical 'stock at hand count' of the previous period</v>
       </c>
       <c r="F2" s="4" t="str">
         <v>Opening balance syringes with needle 1ml</v>
@@ -2798,7 +2798,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I2" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J2" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2818,7 +2818,7 @@
         <v>CVX_OPENING_BALANCE_COLD_BOXES</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>Opening balance equals the physical 'stock on hand count' of the previous period</v>
+        <v>Opening balance equals the physical 'stock at hand count' of the previous period</v>
       </c>
       <c r="F3" s="5" t="str">
         <v>Opening balance cold box</v>
@@ -2830,7 +2830,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I3" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J3" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2862,7 +2862,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I4" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J4" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2894,7 +2894,7 @@
         <v>Percentage</v>
       </c>
       <c r="I5" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J5" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2926,7 +2926,7 @@
         <v>Percentage</v>
       </c>
       <c r="I6" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J6" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2958,7 +2958,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I7" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J7" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2978,7 +2978,7 @@
         <v>CVX_OPENING_BALANCE_VACCINE2_DOSES</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v>Opening balance equals the physical 'stock on hand count' of the previous day</v>
+        <v>Opening balance equals the physical 'stock at hand count' of the previous period</v>
       </c>
       <c r="F8" s="4" t="str">
         <v>Opening balance - Vaccine2 doses</v>
@@ -2990,7 +2990,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I8" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J8" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3022,7 +3022,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I9" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J9" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3054,7 +3054,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I10" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J10" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3086,7 +3086,7 @@
         <v>Percentage</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J11" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3118,7 +3118,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I12" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J12" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3150,7 +3150,7 @@
         <v>Percentage</v>
       </c>
       <c r="I13" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J13" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3182,7 +3182,7 @@
         <v>Percentage</v>
       </c>
       <c r="I14" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J14" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3214,7 +3214,7 @@
         <v>Percentage</v>
       </c>
       <c r="I15" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J15" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3246,7 +3246,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I16" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J16" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3278,7 +3278,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I17" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J17" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3310,7 +3310,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I18" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J18" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3342,7 +3342,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I19" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J19" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3374,7 +3374,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I20" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J20" s="4" t="str">
         <v/>
@@ -3406,7 +3406,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I21" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J21" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3438,7 +3438,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I22" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J22" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3458,7 +3458,7 @@
         <v>CVX_STOCK_DISCREPANCY_VIALS</v>
       </c>
       <c r="E23" s="5" t="str">
-        <v>(Closing balance-Stock on hand)/Stock on hand</v>
+        <v>(Closing balance-Stock on hand)/Stock at hand</v>
       </c>
       <c r="F23" s="5" t="str">
         <v>Closing balance-Stock at hand</v>
@@ -3470,7 +3470,7 @@
         <v>Percentage</v>
       </c>
       <c r="I23" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J23" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3502,7 +3502,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I24" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J24" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3534,7 +3534,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I25" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J25" s="5" t="str">
         <v/>
@@ -3566,7 +3566,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I26" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J26" s="4" t="str">
         <v/>
@@ -3598,7 +3598,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I27" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J27" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3618,7 +3618,7 @@
         <v>CVX_OPENING_BALANCE_VACCINE1_DOSES</v>
       </c>
       <c r="E28" s="4" t="str">
-        <v>Opening balance equals the physical 'stock on hand count of the previous day</v>
+        <v>Opening balance equals the physical 'stock at hand count' of the previous period</v>
       </c>
       <c r="F28" s="4" t="str">
         <v>Opening balance - Vaccine1 doses</v>
@@ -3630,7 +3630,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I28" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J28" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3662,7 +3662,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I29" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J29" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3694,7 +3694,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I30" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J30" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3726,7 +3726,7 @@
         <v>Percentage</v>
       </c>
       <c r="I31" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J31" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3746,7 +3746,7 @@
         <v>CVX_OPENING_BALANCE_VACCINE3_DOSES</v>
       </c>
       <c r="E32" s="4" t="str">
-        <v>Opening balance equals the physical 'stock on hand count' of the previous day</v>
+        <v>Opening balance equals the physical 'stock at hand count' of the previous period</v>
       </c>
       <c r="F32" s="4" t="str">
         <v>Opening balance - Vaccine3 doses</v>
@@ -3758,7 +3758,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I32" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J32" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3790,7 +3790,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I33" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J33" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3822,7 +3822,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I34" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J34" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3854,7 +3854,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I35" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J35" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3886,7 +3886,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I36" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J36" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3918,7 +3918,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I37" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J37" s="5" t="str">
         <v/>
@@ -3950,7 +3950,7 @@
         <v>Percentage</v>
       </c>
       <c r="I38" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J38" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3982,7 +3982,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I39" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J39" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4014,7 +4014,7 @@
         <v>Percentage</v>
       </c>
       <c r="I40" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J40" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4046,7 +4046,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I41" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J41" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4078,7 +4078,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I42" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J42" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4110,7 +4110,7 @@
         <v>Percentage</v>
       </c>
       <c r="I43" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J43" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4142,7 +4142,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I44" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J44" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4174,7 +4174,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I45" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J45" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4206,7 +4206,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I46" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J46" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4238,7 +4238,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I47" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J47" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4270,7 +4270,7 @@
         <v>Percentage</v>
       </c>
       <c r="I48" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J48" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4302,7 +4302,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I49" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J49" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4334,7 +4334,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I50" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J50" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4366,7 +4366,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I51" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J51" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4398,7 +4398,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I52" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J52" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4430,7 +4430,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I53" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J53" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4462,7 +4462,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I54" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J54" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4494,7 +4494,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I55" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J55" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4526,7 +4526,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I56" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J56" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4558,7 +4558,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I57" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J57" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4590,7 +4590,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I58" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J58" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4622,7 +4622,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I59" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J59" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4654,7 +4654,7 @@
         <v>Percentage</v>
       </c>
       <c r="I60" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J60" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4686,7 +4686,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I61" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J61" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4718,7 +4718,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I62" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J62" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4750,7 +4750,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I63" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J63" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4782,7 +4782,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I64" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J64" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4814,7 +4814,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I65" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J65" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4846,7 +4846,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I66" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J66" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4878,7 +4878,7 @@
         <v>Percentage</v>
       </c>
       <c r="I67" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J67" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4910,7 +4910,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I68" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J68" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4942,7 +4942,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I69" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J69" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4974,7 +4974,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I70" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J70" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5006,7 +5006,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I71" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J71" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5038,7 +5038,7 @@
         <v>Percentage</v>
       </c>
       <c r="I72" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J72" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5058,7 +5058,7 @@
         <v>CVX_OPENING_BALANCE_CARDS</v>
       </c>
       <c r="E73" s="5" t="str">
-        <v>Opening balance equals the physical stock on hand count' of the previous period</v>
+        <v>Opening balance equals the physical 'stock at hand count' of the previous period</v>
       </c>
       <c r="F73" s="5" t="str">
         <v>Opening balance vaccination cards</v>
@@ -5070,7 +5070,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I73" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J73" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5102,7 +5102,7 @@
         <v>Percentage</v>
       </c>
       <c r="I74" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J74" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5134,7 +5134,7 @@
         <v>Percentage</v>
       </c>
       <c r="I75" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J75" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5166,7 +5166,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I76" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J76" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5198,7 +5198,7 @@
         <v>Percentage</v>
       </c>
       <c r="I77" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J77" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5230,7 +5230,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I78" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J78" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5262,7 +5262,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I79" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J79" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5294,7 +5294,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I80" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J80" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5326,7 +5326,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I81" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J81" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5358,7 +5358,7 @@
         <v>Percentage</v>
       </c>
       <c r="I82" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J82" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5390,7 +5390,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I83" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J83" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5410,7 +5410,7 @@
         <v>CVX_OPENING_BALANCE_SAFETY_BOXES</v>
       </c>
       <c r="E84" s="4" t="str">
-        <v>Opening balance equals the physical 'stock on hand count' of the previous period</v>
+        <v>Opening balance equals the physical 'stock at hand count' of the previous period</v>
       </c>
       <c r="F84" s="4" t="str">
         <v>Opening balance safety box</v>
@@ -5422,7 +5422,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I84" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J84" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5454,7 +5454,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I85" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J85" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5486,7 +5486,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I86" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J86" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5518,7 +5518,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I87" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J87" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5550,7 +5550,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I88" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J88" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5582,7 +5582,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I89" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J89" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5614,7 +5614,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I90" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J90" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5646,7 +5646,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I91" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J91" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5678,7 +5678,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I92" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J92" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5710,7 +5710,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I93" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J93" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5742,7 +5742,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I94" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J94" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5774,7 +5774,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I95" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J95" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5806,7 +5806,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I96" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J96" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5838,7 +5838,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I97" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J97" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5870,7 +5870,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I98" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J98" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5902,7 +5902,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I99" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J99" s="5" t="str">
         <v/>
@@ -5934,7 +5934,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I100" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J100" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5966,7 +5966,7 @@
         <v>Percentage</v>
       </c>
       <c r="I101" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J101" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5998,7 +5998,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I102" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J102" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6030,7 +6030,7 @@
         <v>Percentage</v>
       </c>
       <c r="I103" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J103" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6062,7 +6062,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I104" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J104" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6094,7 +6094,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I105" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J105" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6126,7 +6126,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I106" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J106" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6158,7 +6158,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I107" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J107" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6190,7 +6190,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I108" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J108" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6222,7 +6222,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I109" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J109" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6254,7 +6254,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I110" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J110" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6286,7 +6286,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I111" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J111" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6318,7 +6318,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I112" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J112" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -6338,7 +6338,7 @@
         <v>CVX_OPENING_BALANCE_VIALS</v>
       </c>
       <c r="E113" s="5" t="str">
-        <v>Opening balance equals the physical 'stock on hand count' of the previous day</v>
+        <v>Opening balance equals the physical 'stock at hand count' of the previous period</v>
       </c>
       <c r="F113" s="5" t="str">
         <v>Opening balance vials</v>
@@ -6350,7 +6350,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I113" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="J113" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -7843,7 +7843,7 @@
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="79.7109375" customWidth="1"/>
+    <col min="4" max="4" width="86.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7875,7 +7875,7 @@
         <v>feQJxQGDpdt</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>COVAX - People given 1st dose</v>
+        <v>COVAX - 1st dose given</v>
       </c>
       <c r="E2" s="4" t="str">
         <v>kif9K3XRSBh</v>
@@ -7892,7 +7892,7 @@
         <v>feQJxQGDpdt</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>COVAX - People given 2+ dose</v>
+        <v>COVAX - 2nd dose given</v>
       </c>
       <c r="E3" s="5" t="str">
         <v>gOf1dLB3r8G</v>
@@ -7909,7 +7909,7 @@
         <v>feQJxQGDpdt</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>COVAX - People given last dose</v>
+        <v>COVAX - Booster given</v>
       </c>
       <c r="E4" s="4" t="str">
         <v>fJzBX7mW5A9</v>
@@ -7926,7 +7926,7 @@
         <v>TUqe8zCkU6V</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>COVAX - Frontline healthcare workers given 2+ dose</v>
+        <v>COVAX - 2nd dose given to HCWs</v>
       </c>
       <c r="E5" s="5" t="str">
         <v>Ly6PaH1qIV3</v>
@@ -7943,7 +7943,7 @@
         <v>TUqe8zCkU6V</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>COVAX - Frontline healthcare workers given 1st dose</v>
+        <v>COVAX - 1st dose given to HCWs</v>
       </c>
       <c r="E6" s="4" t="str">
         <v>FCtGm0HJryo</v>
@@ -7960,7 +7960,7 @@
         <v>TUqe8zCkU6V</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>COVAX - Essential workers given 1st dose</v>
+        <v>COVAX - 1st dose given to essential workers</v>
       </c>
       <c r="E7" s="5" t="str">
         <v>xtorWGRMKCn</v>
@@ -7977,7 +7977,7 @@
         <v>TUqe8zCkU6V</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>COVAX - Essential workers given 2+ dose</v>
+        <v>COVAX - 2nd dose given to essential workers</v>
       </c>
       <c r="E8" s="4" t="str">
         <v>Z8SPWzgXYG5</v>
@@ -7994,7 +7994,7 @@
         <v>TUqe8zCkU6V</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>COVAX - People with at least one underlying medical conditions given 1st dose</v>
+        <v>COVAX - 1st dose given to people with at least one underlying medical conditions</v>
       </c>
       <c r="E9" s="5" t="str">
         <v>BaqWaD6pnbY</v>
@@ -8011,7 +8011,7 @@
         <v>TUqe8zCkU6V</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>COVAX - People with at least one underlying medical conditions given 2+ dose</v>
+        <v>COVAX - 2nd dose given to people with at least one underlying medical conditions</v>
       </c>
       <c r="E10" s="4" t="str">
         <v>leiFl8fMdd3</v>
@@ -8028,7 +8028,7 @@
         <v>TUqe8zCkU6V</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>COVAX - Essential workers given last dose</v>
+        <v>COVAX - Booster dose given to essential workers</v>
       </c>
       <c r="E11" s="5" t="str">
         <v>KhFJj4Qz57c</v>
@@ -8045,7 +8045,7 @@
         <v>TUqe8zCkU6V</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>COVAX - Frontline healthcare workers given last dose</v>
+        <v>COVAX - Booster dose given to HCWs</v>
       </c>
       <c r="E12" s="4" t="str">
         <v>u70rr83wIzM</v>
@@ -8062,7 +8062,7 @@
         <v>TUqe8zCkU6V</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>COVAX - People with at least one underlying medical conditions given last dose</v>
+        <v>COVAX - Booster dose given to people with at least one underlying medical conditions</v>
       </c>
       <c r="E13" s="5" t="str">
         <v>HYYuIK1V5n8</v>
@@ -8079,7 +8079,7 @@
         <v>foPKPuLnZOx</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>COVAX - Doses discarded by reasons</v>
+        <v>COVAX - Doses discarded by reason</v>
       </c>
       <c r="E14" s="4" t="str">
         <v>aGlvT5OwKRZ</v>
@@ -8113,7 +8113,7 @@
         <v>vOnpw5UL45a</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>COVAX - Staff available at centre today</v>
+        <v>COVAX - Staff available at PoC</v>
       </c>
       <c r="E16" s="4" t="str">
         <v>AxmVroGCQZO</v>
@@ -8130,7 +8130,7 @@
         <v>vOnpw5UL45a</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>COVAX - Staff expected at centre today</v>
+        <v>COVAX - Staff expected at PoC</v>
       </c>
       <c r="E17" s="5" t="str">
         <v>FHvsTsdaer9</v>
@@ -8249,7 +8249,7 @@
         <v>kIScH2ovI2E</v>
       </c>
       <c r="D24" s="4" t="str">
-        <v>COVAX - Stockout days vaccine1</v>
+        <v>COVAX - Stockout days vaccine 1</v>
       </c>
       <c r="E24" s="4" t="str">
         <v>VISxgxU3QF1</v>
@@ -8266,7 +8266,7 @@
         <v>kIScH2ovI2E</v>
       </c>
       <c r="D25" s="5" t="str">
-        <v>COVAX - Stockout days vaccine2</v>
+        <v>COVAX - Stockout days vaccine 2</v>
       </c>
       <c r="E25" s="5" t="str">
         <v>suWcEhb54Mz</v>
@@ -8283,7 +8283,7 @@
         <v>kIScH2ovI2E</v>
       </c>
       <c r="D26" s="4" t="str">
-        <v>COVAX - Stockout days vaccine3</v>
+        <v>COVAX - Stockout days vaccine 3</v>
       </c>
       <c r="E26" s="4" t="str">
         <v>sNAklHVNhYj</v>
@@ -8317,7 +8317,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D28" s="4" t="str">
-        <v>COVAX - Discarded cold boxes</v>
+        <v>COVAX - Discarded cold box</v>
       </c>
       <c r="E28" s="4" t="str">
         <v>gHjdt8paeZt</v>
@@ -8334,7 +8334,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D29" s="5" t="str">
-        <v>COVAX - Distributed cold boxes</v>
+        <v>COVAX - Distributed cold box</v>
       </c>
       <c r="E29" s="5" t="str">
         <v>y1TIZ7EacZy</v>
@@ -8351,7 +8351,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D30" s="4" t="str">
-        <v>COVAX - Opening balance cold boxes</v>
+        <v>COVAX - Opening balance cold box</v>
       </c>
       <c r="E30" s="4" t="str">
         <v>e1YlvfQPdTe</v>
@@ -8368,7 +8368,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D31" s="5" t="str">
-        <v>COVAX - Received cold boxes</v>
+        <v>COVAX - Received cold box</v>
       </c>
       <c r="E31" s="5" t="str">
         <v>MhtJeFU1s3g</v>
@@ -8385,7 +8385,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D32" s="4" t="str">
-        <v>COVAX - Redistributed cold boxes</v>
+        <v>COVAX - Redistributed cold box</v>
       </c>
       <c r="E32" s="4" t="str">
         <v>sM3XJvqqU5k</v>
@@ -8402,7 +8402,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D33" s="5" t="str">
-        <v>COVAX - Stock on hand cold boxes</v>
+        <v>COVAX - Stock on hand cold box</v>
       </c>
       <c r="E33" s="5" t="str">
         <v>K1ykBWJNf5C</v>
@@ -8419,7 +8419,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D34" s="4" t="str">
-        <v>COVAX - Stockout days cold boxes</v>
+        <v>COVAX - Stockout days cold box</v>
       </c>
       <c r="E34" s="4" t="str">
         <v>Sq1bNvKm7eE</v>
@@ -8674,7 +8674,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D49" s="5" t="str">
-        <v>COVAX - Discarded safety boxes</v>
+        <v>COVAX - Discarded safety box</v>
       </c>
       <c r="E49" s="5" t="str">
         <v>HlicGU8jEZL</v>
@@ -8691,7 +8691,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D50" s="4" t="str">
-        <v>COVAX - Distributed safety boxes</v>
+        <v>COVAX - Distributed safety box</v>
       </c>
       <c r="E50" s="4" t="str">
         <v>l2tQDaRuqEG</v>
@@ -8708,7 +8708,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D51" s="5" t="str">
-        <v>COVAX - Opening balance safety boxes</v>
+        <v>COVAX - Opening balance safety box</v>
       </c>
       <c r="E51" s="5" t="str">
         <v>maGZEvjJYsL</v>
@@ -8725,7 +8725,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D52" s="4" t="str">
-        <v>COVAX - Received safety boxes</v>
+        <v>COVAX - Received safety box</v>
       </c>
       <c r="E52" s="4" t="str">
         <v>ZdJXThga9s1</v>
@@ -8742,7 +8742,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D53" s="5" t="str">
-        <v>COVAX - Redistributed safety boxes</v>
+        <v>COVAX - Redistributed safety box</v>
       </c>
       <c r="E53" s="5" t="str">
         <v>IA1dFNpYlvJ</v>
@@ -8759,7 +8759,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D54" s="4" t="str">
-        <v>COVAX - Stock on hand safety boxes</v>
+        <v>COVAX - Stock on hand safety box</v>
       </c>
       <c r="E54" s="4" t="str">
         <v>kJnQ1vmDeDe</v>
@@ -8776,7 +8776,7 @@
         <v>Zutn3uE4YnV</v>
       </c>
       <c r="D55" s="5" t="str">
-        <v>COVAX - Stockout days safety boxes</v>
+        <v>COVAX - Stockout days safety box</v>
       </c>
       <c r="E55" s="5" t="str">
         <v>NzVsILZ4qeb</v>
@@ -8934,10 +8934,10 @@
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="79.7109375" customWidth="1"/>
+    <col min="1" max="1" width="86.7109375" customWidth="1"/>
     <col min="2" max="2" width="50.7109375" customWidth="1"/>
     <col min="3" max="3" width="52.7109375" customWidth="1"/>
-    <col min="4" max="4" width="82.7109375" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" customWidth="1"/>
     <col min="5" max="5" width="39.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
@@ -8968,10 +8968,10 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVAX - Doses discarded by reasons</v>
+        <v>COVAX - Doses discarded by reason</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Doses discarded by reasons</v>
+        <v>Doses discarded by reason</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>CVX_DOSES_DISCARDED_BY_REASONS</v>
@@ -8983,7 +8983,7 @@
         <v>Vial condition/Wastage reasons</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G2" s="4" t="str">
         <v>aGlvT5OwKRZ</v>
@@ -8991,22 +8991,22 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVAX - Staff available at centre today</v>
+        <v>COVAX - Staff available at PoC</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Staff available at centre today</v>
+        <v>Staff available at PoC</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>CVX_STAFF_AVAILABLE_AT_CENTRE_TODAY</v>
+        <v>CVX_STAFF_AVAILABLE_AT_POC</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>Total vaccination staff avialable today</v>
+        <v>Total vaccination staff avialable during the reporting period</v>
       </c>
       <c r="E3" s="5" t="str">
         <v>default</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G3" s="5" t="str">
         <v>AxmVroGCQZO</v>
@@ -9014,22 +9014,22 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVAX - People with at least one underlying medical conditions given 1st dose</v>
+        <v>COVAX - 1st dose given to people with at least one underlying medical conditions</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>People with underlying conditions given 1st dose</v>
+        <v>1st dose - People with underlying conditions</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>CVX_PEOPLE_WITH_UNDERLYING_CONDITIONS_1ST_DOSE</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>Total people with underlying medical conditions vaccinated with COVID-19 vaccine</v>
+        <v>People with underlying medical conditions vaccinated with the first dose</v>
       </c>
       <c r="E4" s="4" t="str">
         <v>default</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G4" s="4" t="str">
         <v>BaqWaD6pnbY</v>
@@ -9052,7 +9052,7 @@
         <v>default</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G5" s="5" t="str">
         <v>BeHrxrKVlAB</v>
@@ -9075,7 +9075,7 @@
         <v>Age(&lt;60-60+years)/Sex</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G6" s="4" t="str">
         <v>BHgqoiEc7mS</v>
@@ -9098,7 +9098,7 @@
         <v>default</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G7" s="5" t="str">
         <v>c1NTgV45W8M</v>
@@ -9115,13 +9115,13 @@
         <v>CVX_DISTRIBUTED_VIALS</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>COVID-19 vaccine doses opening balances</v>
+        <v>COVID-19 vaccine vials opening balances</v>
       </c>
       <c r="E8" s="4" t="str">
         <v>COVID19 Vaccine</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G8" s="4" t="str">
         <v>CoCPy5cKxx8</v>
@@ -9144,7 +9144,7 @@
         <v>COVID19 Vaccine</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G9" s="5" t="str">
         <v>DcW8k9WFCoN</v>
@@ -9152,13 +9152,13 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVAX - Opening balance cold boxes</v>
+        <v>COVAX - Opening balance cold box</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Opening balance cold boxes</v>
+        <v>Opening balance cold box</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>CVX_OPENING_BALANCE_COLD_BOXES</v>
+        <v>CVX_OPENING_BALANCE_COLD_BOX</v>
       </c>
       <c r="D10" s="4" t="str">
         <v/>
@@ -9167,7 +9167,7 @@
         <v>default</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G10" s="4" t="str">
         <v>e1YlvfQPdTe</v>
@@ -9190,7 +9190,7 @@
         <v>COVID19 Vaccine</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G11" s="5" t="str">
         <v>ep7EfKNsX3s</v>
@@ -9213,7 +9213,7 @@
         <v>default</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G12" s="4" t="str">
         <v>eTsKBlD7fsX</v>
@@ -9221,22 +9221,22 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>COVAX - Frontline healthcare workers given 1st dose</v>
+        <v>COVAX - 1st dose given to HCWs</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>Frontline healthcare workers given 1st dose</v>
+        <v>1st dose - HCWs</v>
       </c>
       <c r="C13" s="5" t="str">
         <v>CVX_FRONTLINE_HCW_1ST_DOSE</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>Total Healthcare workers vaccinated with COVID-19 vaccine</v>
+        <v>Health Care Workers vaccinated with the first dose</v>
       </c>
       <c r="E13" s="5" t="str">
         <v>default</v>
       </c>
       <c r="F13" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G13" s="5" t="str">
         <v>FCtGm0HJryo</v>
@@ -9244,22 +9244,22 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>COVAX - Staff expected at centre today</v>
+        <v>COVAX - Staff expected at PoC</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Staff expected at centre today</v>
+        <v>Staff expected at PoC</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>CVX_STAFF_EXPECTED_AT_CENTRE_TODAY</v>
+        <v>CVX_STAFF_EXPECTED_AT_PoC</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>Total vaccination staff expected at vaccination centre</v>
+        <v>Total vaccination staff expected at vaccination pont of care during the reporting period</v>
       </c>
       <c r="E14" s="4" t="str">
         <v>default</v>
       </c>
       <c r="F14" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G14" s="4" t="str">
         <v>FHvsTsdaer9</v>
@@ -9267,22 +9267,22 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>COVAX - People given last dose</v>
+        <v>COVAX - Booster given</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>People given last dose</v>
+        <v>Booster dose</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>CVX_PEOPLE_LAST_DOSE</v>
+        <v>CVX_PEOPLE_BOOSTER_DOSE</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>Total people given last dose</v>
+        <v>People receiving the booster dose of COVID-19 vaccine</v>
       </c>
       <c r="E15" s="5" t="str">
         <v>Age(&lt;60-60+years)/Sex/COVID19 Vaccine</v>
       </c>
       <c r="F15" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G15" s="5" t="str">
         <v>fJzBX7mW5A9</v>
@@ -9305,7 +9305,7 @@
         <v>default</v>
       </c>
       <c r="F16" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G16" s="4" t="str">
         <v>fkvWMbUYYvR</v>
@@ -9313,13 +9313,13 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>COVAX - Discarded cold boxes</v>
+        <v>COVAX - Discarded cold box</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Discarded cold boxes</v>
+        <v>Discarded cold box</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>CVX_DISCARDED_COLD_BOXES</v>
+        <v>CVX_DISCARDED_COLD_BOX</v>
       </c>
       <c r="D17" s="5" t="str">
         <v/>
@@ -9328,7 +9328,7 @@
         <v>default</v>
       </c>
       <c r="F17" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G17" s="5" t="str">
         <v>gHjdt8paeZt</v>
@@ -9336,22 +9336,22 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>COVAX - People given 2+ dose</v>
+        <v>COVAX - 2nd dose given</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>People given 2+ dose</v>
+        <v>2nd dose</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>CVX_PEOPLE_2PLUS_DOSE</v>
+        <v>CVX_PEOPLE_2ND_DOSE</v>
       </c>
       <c r="D18" s="4" t="str">
-        <v/>
+        <v>People receiving the second dose of COVID-19 vaccine</v>
       </c>
       <c r="E18" s="4" t="str">
         <v>Age(&lt;60-60+years)/Sex/COVID19 Vaccine</v>
       </c>
       <c r="F18" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G18" s="4" t="str">
         <v>gOf1dLB3r8G</v>
@@ -9368,13 +9368,13 @@
         <v>CVX_AEFIS_BY_VACCINE_AND_SEVERITY</v>
       </c>
       <c r="D19" s="5" t="str">
-        <v>Total number of serious AEFIs reported</v>
+        <v>Serious AEFIs reported</v>
       </c>
       <c r="E19" s="5" t="str">
         <v>COVID19 Vaccine/AEFI Severity</v>
       </c>
       <c r="F19" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G19" s="5" t="str">
         <v>Gw8sB5U5JG3</v>
@@ -9397,7 +9397,7 @@
         <v>default</v>
       </c>
       <c r="F20" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G20" s="4" t="str">
         <v>heMYpVBrakv</v>
@@ -9405,13 +9405,13 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>COVAX - Discarded safety boxes</v>
+        <v>COVAX - Discarded safety box</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>Discarded safety boxes</v>
+        <v>Discarded safety box</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>CVX_DISCARDED_SAFETY_BOXES</v>
+        <v>CVX_DISCARDED_SAFETY_BOX</v>
       </c>
       <c r="D21" s="5" t="str">
         <v/>
@@ -9420,7 +9420,7 @@
         <v>default</v>
       </c>
       <c r="F21" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G21" s="5" t="str">
         <v>HlicGU8jEZL</v>
@@ -9428,22 +9428,22 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>COVAX - People with at least one underlying medical conditions given last dose</v>
+        <v>COVAX - Booster dose given to people with at least one underlying medical conditions</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>People with underlying conditions given last dose</v>
+        <v>Booster - People with underlying conditions</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>CVX_PEOPLE_WITH_UNDERLYING_CONDITIONS_LAST_DOSE</v>
+        <v>CVX_PEOPLE_WITH_UNDERLYING_CONDITIONS_BOOSTER_DOSE</v>
       </c>
       <c r="D22" s="4" t="str">
-        <v>Total people with existing medical conditions given last dose</v>
+        <v>People with underlying medical conditions vaccinated with the booster dose</v>
       </c>
       <c r="E22" s="4" t="str">
         <v>default</v>
       </c>
       <c r="F22" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G22" s="4" t="str">
         <v>HYYuIK1V5n8</v>
@@ -9466,7 +9466,7 @@
         <v>default</v>
       </c>
       <c r="F23" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G23" s="5" t="str">
         <v>i5pakKBw4VC</v>
@@ -9474,13 +9474,13 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>COVAX - Redistributed safety boxes</v>
+        <v>COVAX - Redistributed safety box</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>Redistributed safety boxes</v>
+        <v>Redistributed safety box</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>CVX_REDISTRIBUTED_SAFETY_BOXES</v>
+        <v>CVX_REDISTRIBUTED_SAFETY_BOX</v>
       </c>
       <c r="D24" s="4" t="str">
         <v/>
@@ -9489,7 +9489,7 @@
         <v>default</v>
       </c>
       <c r="F24" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G24" s="4" t="str">
         <v>IA1dFNpYlvJ</v>
@@ -9512,7 +9512,7 @@
         <v>default</v>
       </c>
       <c r="F25" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G25" s="5" t="str">
         <v>jhutPejtr9l</v>
@@ -9535,7 +9535,7 @@
         <v>COVID19 Vaccine</v>
       </c>
       <c r="F26" s="4" t="str">
-        <v>2021-01-27</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G26" s="4" t="str">
         <v>jpHKXTmXBog</v>
@@ -9543,13 +9543,13 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>COVAX - Stock on hand cold boxes</v>
+        <v>COVAX - Stock on hand cold box</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>Stock on hand cold boxes</v>
+        <v>Stock on hand cold box</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>CVX_STOCK_ON_HAND_COLD_BOXES</v>
+        <v>CVX_STOCK_ON_HAND_COLD_BOX</v>
       </c>
       <c r="D27" s="5" t="str">
         <v/>
@@ -9558,7 +9558,7 @@
         <v>default</v>
       </c>
       <c r="F27" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G27" s="5" t="str">
         <v>K1ykBWJNf5C</v>
@@ -9566,22 +9566,22 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>COVAX - Essential workers given last dose</v>
+        <v>COVAX - Booster dose given to essential workers</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>Essential workers given last dose</v>
+        <v>Booster - Essential workers</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>CVX_ESSENTIAL_WORKERS_LAST_DOSE</v>
+        <v>CVX_ESSENTIAL_WORKERS_BOOSTER_DOSE</v>
       </c>
       <c r="D28" s="4" t="str">
-        <v>Total Essential workers given last dose</v>
+        <v>Essential workers who received a booster</v>
       </c>
       <c r="E28" s="4" t="str">
         <v>default</v>
       </c>
       <c r="F28" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G28" s="4" t="str">
         <v>KhFJj4Qz57c</v>
@@ -9589,22 +9589,22 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>COVAX - People given 1st dose</v>
+        <v>COVAX - 1st dose given</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>People given 1st dose</v>
+        <v>1st dose</v>
       </c>
       <c r="C29" s="5" t="str">
         <v>CVX_PEOPLE_1ST_DOSE</v>
       </c>
       <c r="D29" s="5" t="str">
-        <v>Total people vaccinated with COVID-19 vaccine</v>
+        <v>People receiving the first dose of COVID-19 vaccine</v>
       </c>
       <c r="E29" s="5" t="str">
         <v>Age(&lt;60-60+years)/Sex/COVID19 Vaccine</v>
       </c>
       <c r="F29" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G29" s="5" t="str">
         <v>kif9K3XRSBh</v>
@@ -9612,13 +9612,13 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>COVAX - Stock on hand safety boxes</v>
+        <v>COVAX - Stock on hand safety box</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>Stock on hand safety boxes</v>
+        <v>Stock on hand safety box</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v>CVX_STOCK_ON_HAND_SAFETY_BOXES</v>
+        <v>CVX_STOCK_ON_HAND_SAFETY_BOX</v>
       </c>
       <c r="D30" s="4" t="str">
         <v/>
@@ -9627,7 +9627,7 @@
         <v>default</v>
       </c>
       <c r="F30" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G30" s="4" t="str">
         <v>kJnQ1vmDeDe</v>
@@ -9650,7 +9650,7 @@
         <v>default</v>
       </c>
       <c r="F31" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G31" s="5" t="str">
         <v>KWInDqcM0sc</v>
@@ -9658,13 +9658,13 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>COVAX - Distributed safety boxes</v>
+        <v>COVAX - Distributed safety box</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>Distributed safety boxes</v>
+        <v>Distributed safety box</v>
       </c>
       <c r="C32" s="4" t="str">
-        <v>CVX_DISTRIBUTED_SAFETY_BOXES</v>
+        <v>CVX_DISTRIBUTED_SAFETY_BOX</v>
       </c>
       <c r="D32" s="4" t="str">
         <v/>
@@ -9673,7 +9673,7 @@
         <v>default</v>
       </c>
       <c r="F32" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G32" s="4" t="str">
         <v>l2tQDaRuqEG</v>
@@ -9681,22 +9681,22 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>COVAX - People with at least one underlying medical conditions given 2+ dose</v>
+        <v>COVAX - 2nd dose given to people with at least one underlying medical conditions</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>People with underlying conditions given 2+ dose</v>
+        <v>2nd dose - People with underlying conditions</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>CVX_PEOPLE_WITH_UNDERLYING_CONDITIONS_2PLUS_DOSE</v>
+        <v>CVX_PEOPLE_WITH_UNDERLYING_CONDITIONS_2ND_DOSE</v>
       </c>
       <c r="D33" s="5" t="str">
-        <v/>
+        <v>People with underlying medical conditions vaccinated with the second dose</v>
       </c>
       <c r="E33" s="5" t="str">
         <v>default</v>
       </c>
       <c r="F33" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G33" s="5" t="str">
         <v>leiFl8fMdd3</v>
@@ -9704,22 +9704,22 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>COVAX - Frontline healthcare workers given 2+ dose</v>
+        <v>COVAX - 2nd dose given to HCWs</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>Frontline healthcare workers given 2+ dose</v>
+        <v>2nd dose - HCWs</v>
       </c>
       <c r="C34" s="4" t="str">
-        <v>CVX_FRONTLINE_HCW_2PLUS_DOSE</v>
+        <v>CVX_FRONTLINE_HCW_2ND_DOSE</v>
       </c>
       <c r="D34" s="4" t="str">
-        <v/>
+        <v>Health Care Workers who received the second dose</v>
       </c>
       <c r="E34" s="4" t="str">
         <v>default</v>
       </c>
       <c r="F34" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G34" s="4" t="str">
         <v>Ly6PaH1qIV3</v>
@@ -9727,13 +9727,13 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>COVAX - Opening balance safety boxes</v>
+        <v>COVAX - Opening balance safety box</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>Opening balance safety boxes</v>
+        <v>Opening balance safety box</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>CVX_OPENING_BALANCE_SAFETY_BOXES</v>
+        <v>CVX_OPENING_BALANCE_SAFETY_BOX</v>
       </c>
       <c r="D35" s="5" t="str">
         <v/>
@@ -9742,7 +9742,7 @@
         <v>default</v>
       </c>
       <c r="F35" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G35" s="5" t="str">
         <v>maGZEvjJYsL</v>
@@ -9750,13 +9750,13 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>COVAX - Received cold boxes</v>
+        <v>COVAX - Received cold box</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>Received cold boxes</v>
+        <v>Received cold box</v>
       </c>
       <c r="C36" s="4" t="str">
-        <v>CVX_RECEIVED_COLD_BOXES</v>
+        <v>CVX_RECEIVED_COLD_BOX</v>
       </c>
       <c r="D36" s="4" t="str">
         <v/>
@@ -9765,7 +9765,7 @@
         <v>default</v>
       </c>
       <c r="F36" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G36" s="4" t="str">
         <v>MhtJeFU1s3g</v>
@@ -9788,7 +9788,7 @@
         <v>default</v>
       </c>
       <c r="F37" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G37" s="5" t="str">
         <v>mQd64lsZ2Gj</v>
@@ -9811,7 +9811,7 @@
         <v>default</v>
       </c>
       <c r="F38" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G38" s="4" t="str">
         <v>MVmWnSreLrA</v>
@@ -9834,7 +9834,7 @@
         <v>COVID19 Vaccine</v>
       </c>
       <c r="F39" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G39" s="5" t="str">
         <v>Nluny8KPumM</v>
@@ -9842,13 +9842,13 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="str">
-        <v>COVAX - Stockout days safety boxes</v>
+        <v>COVAX - Stockout days safety box</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v>Stockout days safety boxes</v>
+        <v>Stockout days safety box</v>
       </c>
       <c r="C40" s="4" t="str">
-        <v>CVX_STOCKOUT_DAYS_SAFETY_BOXES</v>
+        <v>CVX_STOCKOUT_DAYS_SAFETY_BOX</v>
       </c>
       <c r="D40" s="4" t="str">
         <v/>
@@ -9857,7 +9857,7 @@
         <v>default</v>
       </c>
       <c r="F40" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G40" s="4" t="str">
         <v>NzVsILZ4qeb</v>
@@ -9880,7 +9880,7 @@
         <v>COVID19 Vaccine</v>
       </c>
       <c r="F41" s="5" t="str">
-        <v>2021-01-27</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G41" s="5" t="str">
         <v>oozfHBgiPvP</v>
@@ -9903,7 +9903,7 @@
         <v>default</v>
       </c>
       <c r="F42" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G42" s="4" t="str">
         <v>p9sHAm0M0WF</v>
@@ -9926,7 +9926,7 @@
         <v>default</v>
       </c>
       <c r="F43" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G43" s="5" t="str">
         <v>QFfvrOOhmqw</v>
@@ -9934,13 +9934,13 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="str">
-        <v>COVAX - Redistributed cold boxes</v>
+        <v>COVAX - Redistributed cold box</v>
       </c>
       <c r="B44" s="4" t="str">
-        <v>Redistributed cold boxes</v>
+        <v>Redistributed cold box</v>
       </c>
       <c r="C44" s="4" t="str">
-        <v>CVX_REDISTRIBUTED_COLD_BOXES</v>
+        <v>CVX_REDISTRIBUTED_COLD_BOX</v>
       </c>
       <c r="D44" s="4" t="str">
         <v/>
@@ -9949,7 +9949,7 @@
         <v>default</v>
       </c>
       <c r="F44" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G44" s="4" t="str">
         <v>sM3XJvqqU5k</v>
@@ -9957,10 +9957,10 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="str">
-        <v>COVAX - Stockout days vaccine3</v>
+        <v>COVAX - Stockout days vaccine 3</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>Stockout days vaccine3</v>
+        <v>Stockout days vaccine 3</v>
       </c>
       <c r="C45" s="5" t="str">
         <v>CVX_STOCKOUT_DAYS_VACCINE3</v>
@@ -9972,7 +9972,7 @@
         <v>default</v>
       </c>
       <c r="F45" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G45" s="5" t="str">
         <v>sNAklHVNhYj</v>
@@ -9980,13 +9980,13 @@
     </row>
     <row r="46">
       <c r="A46" s="4" t="str">
-        <v>COVAX - Stockout days cold boxes</v>
+        <v>COVAX - Stockout days cold box</v>
       </c>
       <c r="B46" s="4" t="str">
-        <v>Stockout days cold boxes</v>
+        <v>Stockout days cold box</v>
       </c>
       <c r="C46" s="4" t="str">
-        <v>CVX_STOCKOUT_DAYS_COLD_BOXES</v>
+        <v>CVX_STOCKOUT_DAYS_COLD_BOX</v>
       </c>
       <c r="D46" s="4" t="str">
         <v/>
@@ -9995,7 +9995,7 @@
         <v>default</v>
       </c>
       <c r="F46" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G46" s="4" t="str">
         <v>Sq1bNvKm7eE</v>
@@ -10003,10 +10003,10 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="str">
-        <v>COVAX - Stockout days vaccine2</v>
+        <v>COVAX - Stockout days vaccine 2</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>Stockout days vaccine2</v>
+        <v>Stockout days vaccine 2</v>
       </c>
       <c r="C47" s="5" t="str">
         <v>CVX_STOCKOUT_DAYS_VACCINE2</v>
@@ -10018,7 +10018,7 @@
         <v>default</v>
       </c>
       <c r="F47" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G47" s="5" t="str">
         <v>suWcEhb54Mz</v>
@@ -10026,22 +10026,22 @@
     </row>
     <row r="48">
       <c r="A48" s="4" t="str">
-        <v>COVAX - Frontline healthcare workers given last dose</v>
+        <v>COVAX - Booster dose given to HCWs</v>
       </c>
       <c r="B48" s="4" t="str">
-        <v>Frontline healthcare workers given last dose</v>
+        <v>Booster - HCWs</v>
       </c>
       <c r="C48" s="4" t="str">
-        <v>CVX_FRONTLINE_HCW_LAST_DOSE</v>
+        <v>CVX_FRONTLINE_HCW_BOOSTER_DOSE</v>
       </c>
       <c r="D48" s="4" t="str">
-        <v>Total frontline healthcare workers given last dose</v>
+        <v>Health Care Workers who received a booster</v>
       </c>
       <c r="E48" s="4" t="str">
         <v>default</v>
       </c>
       <c r="F48" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G48" s="4" t="str">
         <v>u70rr83wIzM</v>
@@ -10064,7 +10064,7 @@
         <v>default</v>
       </c>
       <c r="F49" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G49" s="5" t="str">
         <v>UE9gtRQP6RN</v>
@@ -10081,13 +10081,13 @@
         <v>CVX_TARGET_PEOPLE_WITH_EXISTING_MEDICAL_CONDITIONS</v>
       </c>
       <c r="D50" s="4" t="str">
-        <v>Estimated people with at least one underlying medical condition</v>
+        <v>Estimated people with at least one underlying medical condition within the target area</v>
       </c>
       <c r="E50" s="4" t="str">
         <v>default</v>
       </c>
       <c r="F50" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G50" s="4" t="str">
         <v>v2qvl9d2eqz</v>
@@ -10095,10 +10095,10 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="str">
-        <v>COVAX - Stockout days vaccine1</v>
+        <v>COVAX - Stockout days vaccine 1</v>
       </c>
       <c r="B51" s="5" t="str">
-        <v>Stockout days vaccine1</v>
+        <v>Stockout days vaccine 1</v>
       </c>
       <c r="C51" s="5" t="str">
         <v>CVX_STOCKOUT_DAYS_VACCINE1</v>
@@ -10110,7 +10110,7 @@
         <v>default</v>
       </c>
       <c r="F51" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G51" s="5" t="str">
         <v>VISxgxU3QF1</v>
@@ -10127,13 +10127,13 @@
         <v>CVX_TARGET_ESSENTIAL_WORKERS</v>
       </c>
       <c r="D52" s="4" t="str">
-        <v>Estimated essential workers</v>
+        <v>Estimated essential workers within the target area</v>
       </c>
       <c r="E52" s="4" t="str">
         <v>default</v>
       </c>
       <c r="F52" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G52" s="4" t="str">
         <v>vkXAQQDE48p</v>
@@ -10156,7 +10156,7 @@
         <v>default</v>
       </c>
       <c r="F53" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G53" s="5" t="str">
         <v>vThouKg9t52</v>
@@ -10179,7 +10179,7 @@
         <v>COVID19 Vaccine</v>
       </c>
       <c r="F54" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G54" s="4" t="str">
         <v>XgTKGD53X7l</v>
@@ -10187,22 +10187,22 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="str">
-        <v>COVAX - Essential workers given 1st dose</v>
+        <v>COVAX - 1st dose given to essential workers</v>
       </c>
       <c r="B55" s="5" t="str">
-        <v>Essential workers given 1st dose</v>
+        <v>1st dose - Essential workers</v>
       </c>
       <c r="C55" s="5" t="str">
         <v>CVX_ESSENTIAL_WORKERS_1ST_DOSE</v>
       </c>
       <c r="D55" s="5" t="str">
-        <v>Total Essential workers vaccinated with COVID-19 vaccine</v>
+        <v>Essential workers vaccinated with the first dose</v>
       </c>
       <c r="E55" s="5" t="str">
         <v>default</v>
       </c>
       <c r="F55" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G55" s="5" t="str">
         <v>xtorWGRMKCn</v>
@@ -10210,13 +10210,13 @@
     </row>
     <row r="56">
       <c r="A56" s="4" t="str">
-        <v>COVAX - Distributed cold boxes</v>
+        <v>COVAX - Distributed cold box</v>
       </c>
       <c r="B56" s="4" t="str">
-        <v>Distributed cold boxes</v>
+        <v>Distributed cold box</v>
       </c>
       <c r="C56" s="4" t="str">
-        <v>CVX_DISTRIBUTED_COLD_BOXES</v>
+        <v>CVX_DISTRIBUTED_COLD_BOX</v>
       </c>
       <c r="D56" s="4" t="str">
         <v/>
@@ -10225,7 +10225,7 @@
         <v>default</v>
       </c>
       <c r="F56" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G56" s="4" t="str">
         <v>y1TIZ7EacZy</v>
@@ -10242,13 +10242,13 @@
         <v>CVX_TARGET_FRONTLINE_HEALTHCARE_WORKERS</v>
       </c>
       <c r="D57" s="5" t="str">
-        <v/>
+        <v>Estimated health care workers within the target area</v>
       </c>
       <c r="E57" s="5" t="str">
         <v>default</v>
       </c>
       <c r="F57" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G57" s="5" t="str">
         <v>YC0JuESssig</v>
@@ -10256,22 +10256,22 @@
     </row>
     <row r="58">
       <c r="A58" s="4" t="str">
-        <v>COVAX - Essential workers given 2+ dose</v>
+        <v>COVAX - 2nd dose given to essential workers</v>
       </c>
       <c r="B58" s="4" t="str">
-        <v>Essential workers given 2+ dose</v>
+        <v>2nd dose - Essential woekers</v>
       </c>
       <c r="C58" s="4" t="str">
-        <v>CVX_ESSENTIAL_WORKERS_2PLUS_DOSE</v>
+        <v>CVX_ESSENTIAL_WORKERS_2ND_DOSE</v>
       </c>
       <c r="D58" s="4" t="str">
-        <v/>
+        <v>Essential workers who received the second dose</v>
       </c>
       <c r="E58" s="4" t="str">
         <v>default</v>
       </c>
       <c r="F58" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G58" s="4" t="str">
         <v>Z8SPWzgXYG5</v>
@@ -10279,13 +10279,13 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="str">
-        <v>COVAX - Received safety boxes</v>
+        <v>COVAX - Received safety box</v>
       </c>
       <c r="B59" s="5" t="str">
-        <v>Received safety boxes</v>
+        <v>Received safety box</v>
       </c>
       <c r="C59" s="5" t="str">
-        <v>CVX_RECEIVED_SAFETY_BOXES</v>
+        <v>CVX_RECEIVED_SAFETY_BOX</v>
       </c>
       <c r="D59" s="5" t="str">
         <v/>
@@ -10294,7 +10294,7 @@
         <v>default</v>
       </c>
       <c r="F59" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="G59" s="5" t="str">
         <v>ZdJXThga9s1</v>
@@ -10312,7 +10312,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="79.7109375" customWidth="1"/>
+    <col min="2" max="2" width="86.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -10328,7 +10328,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVAX - Doses discarded by reasons</v>
+        <v>COVAX - Doses discarded by reason</v>
       </c>
     </row>
     <row r="3">
@@ -10336,7 +10336,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVAX - Staff available at centre today</v>
+        <v>COVAX - Staff available at PoC</v>
       </c>
     </row>
     <row r="4">
@@ -10344,7 +10344,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAX - People with at least one underlying medical conditions given 1st dose</v>
+        <v>COVAX - 1st dose given to people with at least one underlying medical conditions</v>
       </c>
     </row>
     <row r="5">
@@ -10392,7 +10392,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVAX - Opening balance cold boxes</v>
+        <v>COVAX - Opening balance cold box</v>
       </c>
     </row>
     <row r="11">
@@ -10416,7 +10416,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVAX - Frontline healthcare workers given 1st dose</v>
+        <v>COVAX - 1st dose given to HCWs</v>
       </c>
     </row>
     <row r="14">
@@ -10424,7 +10424,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVAX - Staff expected at centre today</v>
+        <v>COVAX - Staff expected at PoC</v>
       </c>
     </row>
     <row r="15">
@@ -10432,7 +10432,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVAX - People given last dose</v>
+        <v>COVAX - Booster given</v>
       </c>
     </row>
     <row r="16">
@@ -10448,7 +10448,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>COVAX - Discarded cold boxes</v>
+        <v>COVAX - Discarded cold box</v>
       </c>
     </row>
     <row r="18">
@@ -10456,7 +10456,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>COVAX - People given 2+ dose</v>
+        <v>COVAX - 2nd dose given</v>
       </c>
     </row>
     <row r="19">
@@ -10480,7 +10480,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>COVAX - Discarded safety boxes</v>
+        <v>COVAX - Discarded safety box</v>
       </c>
     </row>
     <row r="22">
@@ -10488,7 +10488,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>COVAX - People with at least one underlying medical conditions given last dose</v>
+        <v>COVAX - Booster dose given to people with at least one underlying medical conditions</v>
       </c>
     </row>
     <row r="23">
@@ -10504,7 +10504,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>COVAX - Redistributed safety boxes</v>
+        <v>COVAX - Redistributed safety box</v>
       </c>
     </row>
     <row r="25">
@@ -10528,7 +10528,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>COVAX - Stock on hand cold boxes</v>
+        <v>COVAX - Stock on hand cold box</v>
       </c>
     </row>
     <row r="28">
@@ -10536,7 +10536,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>COVAX - Essential workers given last dose</v>
+        <v>COVAX - Booster dose given to essential workers</v>
       </c>
     </row>
     <row r="29">
@@ -10544,7 +10544,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>COVAX - People given 1st dose</v>
+        <v>COVAX - 1st dose given</v>
       </c>
     </row>
     <row r="30">
@@ -10552,7 +10552,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>COVAX - Stock on hand safety boxes</v>
+        <v>COVAX - Stock on hand safety box</v>
       </c>
     </row>
     <row r="31">
@@ -10568,7 +10568,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>COVAX - Distributed safety boxes</v>
+        <v>COVAX - Distributed safety box</v>
       </c>
     </row>
     <row r="33">
@@ -10576,7 +10576,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>COVAX - People with at least one underlying medical conditions given 2+ dose</v>
+        <v>COVAX - 2nd dose given to people with at least one underlying medical conditions</v>
       </c>
     </row>
     <row r="34">
@@ -10584,7 +10584,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>COVAX - Frontline healthcare workers given 2+ dose</v>
+        <v>COVAX - 2nd dose given to HCWs</v>
       </c>
     </row>
     <row r="35">
@@ -10592,7 +10592,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>COVAX - Opening balance safety boxes</v>
+        <v>COVAX - Opening balance safety box</v>
       </c>
     </row>
     <row r="36">
@@ -10600,7 +10600,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>COVAX - Received cold boxes</v>
+        <v>COVAX - Received cold box</v>
       </c>
     </row>
     <row r="37">
@@ -10632,7 +10632,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v>COVAX - Stockout days safety boxes</v>
+        <v>COVAX - Stockout days safety box</v>
       </c>
     </row>
     <row r="41">
@@ -10656,7 +10656,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B43" s="5" t="str">
-        <v>COVAX - Redistributed cold boxes</v>
+        <v>COVAX - Redistributed cold box</v>
       </c>
     </row>
     <row r="44">
@@ -10664,7 +10664,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B44" s="4" t="str">
-        <v>COVAX - Stockout days vaccine3</v>
+        <v>COVAX - Stockout days vaccine 3</v>
       </c>
     </row>
     <row r="45">
@@ -10672,7 +10672,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>COVAX - Stockout days cold boxes</v>
+        <v>COVAX - Stockout days cold box</v>
       </c>
     </row>
     <row r="46">
@@ -10680,7 +10680,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B46" s="4" t="str">
-        <v>COVAX - Stockout days vaccine2</v>
+        <v>COVAX - Stockout days vaccine 2</v>
       </c>
     </row>
     <row r="47">
@@ -10688,7 +10688,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>COVAX - Frontline healthcare workers given last dose</v>
+        <v>COVAX - Booster dose given to HCWs</v>
       </c>
     </row>
     <row r="48">
@@ -10712,7 +10712,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B50" s="4" t="str">
-        <v>COVAX - Stockout days vaccine1</v>
+        <v>COVAX - Stockout days vaccine 1</v>
       </c>
     </row>
     <row r="51">
@@ -10744,7 +10744,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B54" s="4" t="str">
-        <v>COVAX - Essential workers given 1st dose</v>
+        <v>COVAX - 1st dose given to essential workers</v>
       </c>
     </row>
     <row r="55">
@@ -10752,7 +10752,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B55" s="5" t="str">
-        <v>COVAX - Distributed cold boxes</v>
+        <v>COVAX - Distributed cold box</v>
       </c>
     </row>
     <row r="56">
@@ -10768,7 +10768,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B57" s="5" t="str">
-        <v>COVAX - Essential workers given 2+ dose</v>
+        <v>COVAX - 2nd dose given to essential workers</v>
       </c>
     </row>
     <row r="58">
@@ -10776,7 +10776,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B58" s="4" t="str">
-        <v>COVAX - Received safety boxes</v>
+        <v>COVAX - Received safety box</v>
       </c>
     </row>
   </sheetData>

</xml_diff>